<commit_message>
4th Commit | Important Commit
- Changing exports to zero (Now the model will account exports and imports only by net food and feed)
- Started adding grass crop
</commit_message>
<xml_diff>
--- a/InputFiles_CBW/CommonDataLabels.xlsx
+++ b/InputFiles_CBW/CommonDataLabels.xlsx
@@ -40749,8 +40749,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050CB5C7BD841A746A008EF8990FEF8A1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="04f0adbf5da449b72a87907c36bfe402">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d795cf93-200f-4322-ae4e-3af3c2bc7b07" xmlns:ns3="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e4044cd58a51a52832fd40a04c970f" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050CB5C7BD841A746A008EF8990FEF8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcac96711073587df0b68b080c708180">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d795cf93-200f-4322-ae4e-3af3c2bc7b07" xmlns:ns3="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98209c71c39a5a5ad103d397a60c957b" ns2:_="" ns3:_="">
     <xsd:import namespace="d795cf93-200f-4322-ae4e-3af3c2bc7b07"/>
     <xsd:import namespace="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59"/>
     <xsd:element name="properties">
@@ -40773,6 +40773,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -40843,6 +40844,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" elementFormDefault="qualified">
@@ -41005,7 +41011,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BE64500-627D-4B8E-ADA6-FC4B29D9F9FD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DB70681-A8C9-40EE-A6DD-9CA96E17CA7F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>